<commit_message>
feat: realização do primeiro exercício
</commit_message>
<xml_diff>
--- a/03-back-end/bloco-21-funcoes-sql-joins-e-normalizacao/dia-03-transformando-ideias-em-um-modelo-de-banco-de-dados/exercise-01/requisito-01.xlsx
+++ b/03-back-end/bloco-21-funcoes-sql-joins-e-normalizacao/dia-03-transformando-ideias-em-um-modelo-de-banco-de-dados/exercise-01/requisito-01.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/guilhermefernandes/TRYBE/repositorios-github/trybe-exercicios/03-back-end/bloco-21-funcoes-sql-joins-e-normalizacao/dia-03-transformando-ideias-em-um-modelo-de-banco-de-dados/exercise-01/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE1D85FF-694C-174E-9386-4CF509DE8CD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58AE2FC2-9F00-264A-99CB-6690EEF47B51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10000" yWindow="1240" windowWidth="27960" windowHeight="17360" xr2:uid="{580F4324-5D1B-A343-8ADC-F20465F88DAB}"/>
   </bookViews>
@@ -211,9 +211,6 @@
     <xf numFmtId="22" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="22" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="22" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -222,6 +219,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="22" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="60% - Ênfase3" xfId="1" builtinId="40"/>
@@ -540,7 +540,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -554,23 +554,23 @@
     <col min="8" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="8" customFormat="1" ht="20" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:6" s="7" customFormat="1" ht="20" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="6" t="s">
         <v>4</v>
       </c>
     </row>
@@ -610,7 +610,7 @@
       <c r="E3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="8">
         <v>43866</v>
       </c>
     </row>
@@ -655,16 +655,16 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="F6" s="5"/>
-    </row>
-    <row r="7" spans="1:6" s="8" customFormat="1" ht="20" x14ac:dyDescent="0.2">
-      <c r="A7" s="7" t="s">
+      <c r="F6" s="4"/>
+    </row>
+    <row r="7" spans="1:6" s="7" customFormat="1" ht="20" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="6" t="s">
         <v>5</v>
       </c>
     </row>
@@ -713,10 +713,10 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="20" x14ac:dyDescent="0.2">
-      <c r="A12" s="6">
+      <c r="A12" s="5">
         <v>5</v>
       </c>
-      <c r="B12" s="6">
+      <c r="B12" s="5">
         <v>14</v>
       </c>
       <c r="C12" s="2" t="s">
@@ -724,10 +724,10 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="20" x14ac:dyDescent="0.2">
-      <c r="A13" s="6">
+      <c r="A13" s="5">
         <v>6</v>
       </c>
-      <c r="B13" s="6">
+      <c r="B13" s="5">
         <v>15</v>
       </c>
       <c r="C13" s="2" t="s">

</xml_diff>